<commit_message>
06.06.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/June/All Details/04.06.2020/MC Balance Transfer June 2020.xlsx
+++ b/2020/June/All Details/04.06.2020/MC Balance Transfer June 2020.xlsx
@@ -1105,7 +1105,7 @@
         <xdr:cNvPr id="1317" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1117,7 +1117,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1140,14 +1140,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1455,9 +1455,9 @@
   <dimension ref="A1:BI231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="E92" sqref="E92"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1970,17 +1970,17 @@
         <v>81</v>
       </c>
       <c r="B8" s="2">
-        <v>932480</v>
+        <v>929570</v>
       </c>
       <c r="C8" s="2">
-        <v>944055</v>
+        <v>941145</v>
       </c>
       <c r="D8" s="2">
         <v>1365</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>945420</v>
+        <v>942510</v>
       </c>
       <c r="F8" s="67"/>
       <c r="G8" s="17"/>
@@ -3677,11 +3677,11 @@
       </c>
       <c r="B33" s="2">
         <f>SUM(B5:B32)</f>
-        <v>2474430</v>
+        <v>2471520</v>
       </c>
       <c r="C33" s="2">
         <f>SUM(C5:C32)</f>
-        <v>2435635</v>
+        <v>2432725</v>
       </c>
       <c r="D33" s="2">
         <f>SUM(D5:D32)</f>
@@ -3689,7 +3689,7 @@
       </c>
       <c r="E33" s="2">
         <f>SUM(E5:E32)</f>
-        <v>2439770</v>
+        <v>2436860</v>
       </c>
       <c r="F33" s="67">
         <f>B33-E33</f>

</xml_diff>